<commit_message>
added calc for number of boards
</commit_message>
<xml_diff>
--- a/Fabrication_and_Assembly_Files/ParallelCS_Assembly_March_2019/BOM2019..xlsx
+++ b/Fabrication_and_Assembly_Files/ParallelCS_Assembly_March_2019/BOM2019..xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djave\Parallel_CS_Altium\Fabrication_and_Assembly_Files\Assembly_Files_Parallel_CS_April_18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Parallel_CS_Altium\Fabrication_and_Assembly_Files\ParallelCS_Assembly_March_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{943D78C2-168F-41B3-A70F-95894B3433D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C57A16A-04D5-4EB9-912B-7D487BD6D4DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
   <si>
     <t xml:space="preserve">Bill of Material for </t>
   </si>
@@ -278,12 +285,21 @@
   </si>
   <si>
     <t>Change in part number confirmed</t>
+  </si>
+  <si>
+    <t>Min Order</t>
+  </si>
+  <si>
+    <t>Boards</t>
+  </si>
+  <si>
+    <t>James Ordered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1142,37 +1158,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.46484375" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="4" max="4" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.73046875" customWidth="1"/>
+    <col min="6" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.19921875" customWidth="1"/>
+    <col min="9" max="9" width="7.46484375" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1192,19 +1217,25 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
         <v>58</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>60</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>79</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1223,11 +1254,15 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>ROUNDUP(1.05*(C6*$G$3),0)</f>
+        <v>384</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1246,15 +1281,19 @@
       <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7">
+        <f t="shared" ref="G7:G28" si="0">ROUNDUP(1.05*(C7*$G$3),0)</f>
+        <v>252</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="2">
         <v>2112793</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1273,15 +1312,19 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="2">
         <v>1575900</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1300,11 +1343,15 @@
       <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1323,11 +1370,15 @@
       <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1346,11 +1397,15 @@
       <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1369,11 +1424,15 @@
       <c r="F12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1392,11 +1451,15 @@
       <c r="F13" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1415,15 +1478,19 @@
       <c r="F14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="2">
         <v>2694242</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1442,11 +1509,15 @@
       <c r="F15" t="s">
         <v>9</v>
       </c>
-      <c r="G15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1465,11 +1536,15 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>330</v>
       </c>
@@ -1488,11 +1563,15 @@
       <c r="F17" t="s">
         <v>9</v>
       </c>
-      <c r="G17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1511,11 +1590,15 @@
       <c r="F18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1534,18 +1617,22 @@
       <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="G19" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="2">
         <v>2920485</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" t="s">
+      <c r="K19" s="2"/>
+      <c r="L19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1564,15 +1651,19 @@
       <c r="F20" t="s">
         <v>13</v>
       </c>
-      <c r="G20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="2">
         <v>2484006</v>
       </c>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>715</v>
       </c>
@@ -1591,15 +1682,19 @@
       <c r="F21" t="s">
         <v>13</v>
       </c>
-      <c r="G21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="2">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="2">
         <v>2303536</v>
       </c>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1618,15 +1713,19 @@
       <c r="F22" t="s">
         <v>13</v>
       </c>
-      <c r="G22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="2">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="2">
         <v>1581966</v>
       </c>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1645,17 +1744,21 @@
       <c r="F23" t="s">
         <v>13</v>
       </c>
-      <c r="G23" t="s">
-        <v>63</v>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="I23" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" t="s">
         <v>84</v>
       </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1674,14 +1777,18 @@
       <c r="F24" t="s">
         <v>13</v>
       </c>
-      <c r="G24" t="s">
-        <v>63</v>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="I24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1700,15 +1807,19 @@
       <c r="F25" t="s">
         <v>13</v>
       </c>
-      <c r="G25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="2">
         <v>1332158</v>
       </c>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1727,14 +1838,18 @@
       <c r="F26" t="s">
         <v>13</v>
       </c>
-      <c r="G26" t="s">
-        <v>63</v>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>126</v>
       </c>
       <c r="I26" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1753,14 +1868,18 @@
       <c r="F27" t="s">
         <v>13</v>
       </c>
-      <c r="G27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="2">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="2">
         <v>1328309</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1776,17 +1895,21 @@
       <c r="F28" t="s">
         <v>13</v>
       </c>
-      <c r="G28" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" s="2">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I28" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="2">
         <v>1568026</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>56</v>
       </c>
@@ -1795,7 +1918,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>57</v>
       </c>

</xml_diff>